<commit_message>
Updated excel code profile with more accurate values
</commit_message>
<xml_diff>
--- a/RoboBee_Algorithm_Code_Profile.xlsx
+++ b/RoboBee_Algorithm_Code_Profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlarc\OneDrive\Desktop\Robo Bee project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80413F55-4874-4364-B3BE-CB5720FAFC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B466712E-8317-44D1-A654-20B4B294D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="0" windowWidth="22260" windowHeight="12336" tabRatio="354" xr2:uid="{E598E94E-7A81-4F82-8BF3-06B37786DBA6}"/>
+    <workbookView xWindow="28740" yWindow="0" windowWidth="14100" windowHeight="15585" tabRatio="354" xr2:uid="{E598E94E-7A81-4F82-8BF3-06B37786DBA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Total instructions</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Identity() / 3</t>
-  </si>
-  <si>
-    <t>cos() / 176</t>
-  </si>
-  <si>
-    <t>sin() / 192</t>
   </si>
   <si>
     <t>completeOrthogonalDecomposition() / 1</t>
@@ -129,9 +123,6 @@
     <t>row() / 1197</t>
   </si>
   <si>
-    <t>transpose() / 1201</t>
-  </si>
-  <si>
     <t>head() / 1</t>
   </si>
   <si>
@@ -222,20 +213,43 @@
     <t>getRMSE() / 2</t>
   </si>
   <si>
-    <t>time to run program * clockspeed</t>
-  </si>
-  <si>
     <t>Use look up table instead of sin cos functions</t>
   </si>
   <si>
     <t>Memory for program (Kilobytes)</t>
-  </si>
-  <si>
-    <t>Number of cycles per program</t>
   </si>
   <si>
     <t>Nested Function / Calls
 (what calls what?)</t>
+  </si>
+  <si>
+    <t>Cycles per program
+(48 Mhz M0 Arm Cortex)</t>
+  </si>
+  <si>
+    <t>Cycles per datapoint
+(48 Mhz M0 Arm Cortex)</t>
+  </si>
+  <si>
+    <t>wall clock time to run program * clockspeed</t>
+  </si>
+  <si>
+    <t>cos() / 210,320</t>
+  </si>
+  <si>
+    <t>176 * 1195</t>
+  </si>
+  <si>
+    <t>192 * 1195</t>
+  </si>
+  <si>
+    <t>sin() / 229,440</t>
+  </si>
+  <si>
+    <t>6 * 1195</t>
+  </si>
+  <si>
+    <t>transpose() / 7,170</t>
   </si>
 </sst>
 </file>
@@ -383,7 +397,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -419,6 +433,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -766,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240AD737-D13A-4082-9D0B-AB1F50C973EC}">
-  <dimension ref="B1:L27"/>
+  <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -782,49 +799,57 @@
     <col min="6" max="6" width="22" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.88671875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.21875" style="1" customWidth="1"/>
-    <col min="9" max="12" width="13.33203125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="10" width="13.33203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="15.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="14"/>
+    <row r="1" spans="2:13" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="15"/>
       <c r="F1" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -835,26 +860,27 @@
         <v>12</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2">
         <v>539.96</v>
       </c>
       <c r="K3" s="12">
-        <f>(60 * 2 *POWER(10,9)) / 1195</f>
-        <v>100418410.041841</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <f>(0.36 * 48 *POWER(10,6)) / 1195</f>
+        <v>14460.251046025105</v>
+      </c>
+      <c r="L3" s="13">
+        <f>0.36 * 48 *POWER(10,6)</f>
+        <v>17280000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -865,76 +891,85 @@
         <v>13</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="E5" s="6" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E6" s="6" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -942,19 +977,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -962,116 +997,116 @@
         <v>1</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E11" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14"/>
       <c r="E14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E15" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E16" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E17" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E19" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E20" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E21" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E22" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E23" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E24" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E25" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E26" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="5:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E27" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>